<commit_message>
add Details, add description:Cat,Dram,Perm,Prov, building AccountForm
</commit_message>
<xml_diff>
--- a/Documents/2016-2017-Java-PhieuVanDap-DAQuanLyBanHang.xlsx
+++ b/Documents/2016-2017-Java-PhieuVanDap-DAQuanLyBanHang.xlsx
@@ -1729,8 +1729,8 @@
   <dimension ref="A1:IV45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1894,7 +1894,9 @@
       <c r="E12" s="19">
         <v>2.75</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="9">
+        <v>2.75</v>
+      </c>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="36.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -2015,7 +2017,9 @@
       <c r="E21" s="20">
         <v>0.25</v>
       </c>
-      <c r="F21" s="9"/>
+      <c r="F21" s="9">
+        <v>0.25</v>
+      </c>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" ht="36.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -2073,7 +2077,9 @@
       <c r="E25" s="19">
         <v>3.25</v>
       </c>
-      <c r="F25" s="9"/>
+      <c r="F25" s="9">
+        <v>1</v>
+      </c>
       <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.2">
@@ -2118,7 +2124,9 @@
       <c r="E28" s="20">
         <v>0.25</v>
       </c>
-      <c r="F28" s="9"/>
+      <c r="F28" s="9">
+        <v>0.25</v>
+      </c>
       <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.2">
@@ -2242,7 +2250,9 @@
       <c r="E36" s="19">
         <v>3.5</v>
       </c>
-      <c r="F36" s="9"/>
+      <c r="F36" s="9">
+        <v>0.25</v>
+      </c>
       <c r="G36" s="9"/>
     </row>
     <row r="37" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.2">
@@ -2294,7 +2304,9 @@
       <c r="E40" s="20">
         <v>0.25</v>
       </c>
-      <c r="F40" s="9"/>
+      <c r="F40" s="9">
+        <v>0.25</v>
+      </c>
       <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.2">
@@ -2346,7 +2358,9 @@
       <c r="E44" s="19">
         <v>0.5</v>
       </c>
-      <c r="F44" s="9"/>
+      <c r="F44" s="9">
+        <v>0.5</v>
+      </c>
       <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>